<commit_message>
version minus 7 building
</commit_message>
<xml_diff>
--- a/ReportApi/bin/Debug/net4.8.1/BSUMBILLMASTER.xlsx
+++ b/ReportApi/bin/Debug/net4.8.1/BSUMBILLMASTER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PVV\PvvReportAPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sysadmin\Documents\ReportApi\ReportApi\bin\Debug\net4.8.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155124EE-D24A-4D01-9D76-D894DA40EB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23CBB9B-D307-4007-AA04-3E7BA584D86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1530" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>หนังสือแจ้งค่าไฟฟ้า</t>
   </si>
@@ -108,12 +108,6 @@
     <t>รวมเงินที่ต้องชำระ</t>
   </si>
   <si>
-    <t>โปรดชำระภายในวันที่</t>
-  </si>
-  <si>
-    <t>20 พฤศจิกายน 2565</t>
-  </si>
-  <si>
     <t>หมายเหตุ</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>ตำแหน่ง......................................................</t>
   </si>
   <si>
-    <t xml:space="preserve"> ห้าแสนหกพันหกร้อยสี่สิบห้าบาทสี่สิบเอ็ดสตางค์</t>
-  </si>
-  <si>
     <t>มหาวิทยาลัยมหิดล</t>
   </si>
   <si>
@@ -157,6 +148,12 @@
   </si>
   <si>
     <t>ค่าอัตราต่อหน่วยลด 46.1% (บาท)</t>
+  </si>
+  <si>
+    <t>โปรดชำระภายใน 30(สามสิบ) วันนับตั้งแต่ได้รับใบแจ้งหนี้ค่าพลังงานไฟฟ้า</t>
+  </si>
+  <si>
+    <t xml:space="preserve">รวมเงินที่ต้องชำระ </t>
   </si>
 </sst>
 </file>
@@ -168,7 +165,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="[$-107041E]d\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +177,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,27 +359,30 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,7 +736,7 @@
   <dimension ref="A2:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C23" sqref="C23:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,19 +753,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G4" s="1"/>
@@ -767,7 +775,7 @@
       </c>
       <c r="J4" s="18">
         <f ca="1">NOW()</f>
-        <v>45175.472039120374</v>
+        <v>45274.716774652778</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -788,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H7" s="2"/>
       <c r="J7" t="s">
@@ -796,14 +804,14 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="26"/>
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
@@ -821,14 +829,14 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="3">
         <v>250613870</v>
       </c>
@@ -853,15 +861,15 @@
         <v>17</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="26"/>
+      <c r="H13" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="24"/>
       <c r="J13" s="11">
         <v>3</v>
       </c>
@@ -879,17 +887,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="21">
-        <f>D14-E14</f>
         <v>100</v>
       </c>
       <c r="G14" s="7">
         <f>F14*(J13-J14)</f>
         <v>100</v>
       </c>
-      <c r="H14" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="26"/>
+      <c r="H14" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="24"/>
       <c r="J14" s="20">
         <v>2</v>
       </c>
@@ -903,8 +910,8 @@
       <c r="E15" s="12"/>
       <c r="F15" s="15"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="26"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -919,10 +926,10 @@
         <f>G14</f>
         <v>100</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="26"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="11">
         <f>G16</f>
         <v>100</v>
@@ -941,116 +948,105 @@
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
+      <c r="B19" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="30" t="str">
+        <f>IF(J16="","",BAHTTEXT(J16))</f>
+        <v>หนึ่งร้อยบาทถ้วน</v>
+      </c>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+    </row>
+    <row r="26" spans="2:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="22" t="s">
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="H26" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+    </row>
+    <row r="27" spans="2:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H25" s="23" t="s">
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="H27" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-    </row>
-    <row r="26" spans="2:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="s">
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+    </row>
+    <row r="28" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="H26" s="22" t="s">
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="H28" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-    </row>
-    <row r="27" spans="2:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+    </row>
+    <row r="29" spans="2:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="H27" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-    </row>
-    <row r="28" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="H28" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-    </row>
-    <row r="29" spans="2:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="B26:E26"/>
@@ -1059,6 +1055,19 @@
     <mergeCell ref="H27:J27"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="H28:J28"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
edit from makam comment
</commit_message>
<xml_diff>
--- a/ReportApi/bin/Debug/net4.8.1/BSUMBILLMASTER.xlsx
+++ b/ReportApi/bin/Debug/net4.8.1/BSUMBILLMASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sysadmin\Documents\ReportApi\ReportApi\bin\Debug\net4.8.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23CBB9B-D307-4007-AA04-3E7BA584D86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77976582-908F-4B43-9F67-ADCA9E4C557B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1530" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="30" windowWidth="23970" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -359,30 +359,30 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,7 +736,7 @@
   <dimension ref="A2:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:J23"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,19 +753,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G4" s="1"/>
@@ -775,7 +775,7 @@
       </c>
       <c r="J4" s="18">
         <f ca="1">NOW()</f>
-        <v>45274.716774652778</v>
+        <v>45279.601706944442</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -804,14 +804,14 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="26"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
@@ -829,14 +829,14 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="25" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="26"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="3">
         <v>250613870</v>
       </c>
@@ -866,10 +866,10 @@
       <c r="G13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="27"/>
       <c r="J13" s="11">
         <v>3</v>
       </c>
@@ -890,13 +890,13 @@
         <v>100</v>
       </c>
       <c r="G14" s="7">
-        <f>F14*(J13-J14)</f>
+        <f>(F14*J13)-(F14*J14)</f>
         <v>100</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="27"/>
       <c r="J14" s="20">
         <v>2</v>
       </c>
@@ -910,8 +910,8 @@
       <c r="E15" s="12"/>
       <c r="F15" s="15"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
       <c r="J15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -926,10 +926,10 @@
         <f>G14</f>
         <v>100</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="24"/>
+      <c r="I16" s="27"/>
       <c r="J16" s="11">
         <f>G16</f>
         <v>100</v>
@@ -948,31 +948,31 @@
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="30" t="str">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25" t="str">
         <f>IF(J16="","",BAHTTEXT(J16))</f>
         <v>หนึ่งร้อยบาทถ้วน</v>
       </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -980,73 +980,86 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
     </row>
     <row r="26" spans="2:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="H26" s="28" t="s">
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="H26" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" spans="2:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="H27" s="28" t="s">
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="H27" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="H28" s="28" t="s">
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="H28" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="2:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D20:H20"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="B26:E26"/>
@@ -1055,19 +1068,6 @@
     <mergeCell ref="H27:J27"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="H28:J28"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>